<commit_message>
updating to run reverse OM selex
</commit_message>
<xml_diff>
--- a/input/OM_EM_Scenarios_v3.xlsx
+++ b/input/OM_EM_Scenarios_v3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Fleet_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67512FA3-BFE6-D34C-9DDA-69C2526CB09A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A43F9406-D172-124D-9A88-130C206F33E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{7DE04263-F460-4046-B781-542FFAD9869D}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{7DE04263-F460-4046-B781-542FFAD9869D}"/>
   </bookViews>
   <sheets>
     <sheet name="OM" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="179">
   <si>
     <t>Fl_1_Ftype</t>
   </si>
@@ -562,6 +562,24 @@
   </si>
   <si>
     <t>Int_1Fl_Gam_SP_1.0</t>
+  </si>
+  <si>
+    <t>Fast_LL_High_Rev</t>
+  </si>
+  <si>
+    <t>Fast_GL_O_High_Rev</t>
+  </si>
+  <si>
+    <t>Slow_LL_High_Rev</t>
+  </si>
+  <si>
+    <t>Slow_GL_O_High_Rev</t>
+  </si>
+  <si>
+    <t>Fast_GL_Y_High_Rev</t>
+  </si>
+  <si>
+    <t>Slow_GL_Y_High_Rev</t>
   </si>
 </sst>
 </file>
@@ -936,8 +954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3458753E-37AB-3F45-AB3E-5A0862A1384B}">
   <dimension ref="A1:AA27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O8" sqref="O8:P13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2046,30 +2064,513 @@
       </c>
     </row>
     <row r="14" spans="1:27" ht="20" x14ac:dyDescent="0.2">
-      <c r="J14" s="2"/>
+      <c r="A14" t="s">
+        <v>173</v>
+      </c>
+      <c r="B14">
+        <v>51</v>
+      </c>
+      <c r="C14">
+        <v>30</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14">
+        <v>0.108</v>
+      </c>
+      <c r="H14">
+        <v>5.6842109999999998E-3</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0.76670000000000005</v>
+      </c>
+      <c r="K14">
+        <v>100</v>
+      </c>
+      <c r="L14">
+        <v>100</v>
+      </c>
+      <c r="M14">
+        <v>100</v>
+      </c>
+      <c r="N14">
+        <v>0.2</v>
+      </c>
+      <c r="O14">
+        <v>50</v>
+      </c>
+      <c r="P14">
+        <v>50</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>10</v>
+      </c>
+      <c r="R14" t="s">
+        <v>10</v>
+      </c>
+      <c r="S14">
+        <v>8.5</v>
+      </c>
+      <c r="T14">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="U14">
+        <v>10.5</v>
+      </c>
+      <c r="V14">
+        <v>1.25</v>
+      </c>
+      <c r="W14">
+        <v>3.5</v>
+      </c>
+      <c r="X14">
+        <v>0.65</v>
+      </c>
+      <c r="Y14">
+        <v>5.5</v>
+      </c>
+      <c r="Z14">
+        <v>0.75</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="15" spans="1:27" ht="20" x14ac:dyDescent="0.2">
-      <c r="J15" s="2"/>
+      <c r="A15" t="s">
+        <v>174</v>
+      </c>
+      <c r="B15">
+        <v>51</v>
+      </c>
+      <c r="C15">
+        <v>30</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15">
+        <v>0.108</v>
+      </c>
+      <c r="H15">
+        <v>5.6842109999999998E-3</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0.76670000000000005</v>
+      </c>
+      <c r="K15">
+        <v>100</v>
+      </c>
+      <c r="L15">
+        <v>100</v>
+      </c>
+      <c r="M15">
+        <v>100</v>
+      </c>
+      <c r="N15">
+        <v>0.2</v>
+      </c>
+      <c r="O15">
+        <v>50</v>
+      </c>
+      <c r="P15">
+        <v>50</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>11</v>
+      </c>
+      <c r="R15" t="s">
+        <v>10</v>
+      </c>
+      <c r="S15">
+        <v>15.5</v>
+      </c>
+      <c r="T15">
+        <v>8</v>
+      </c>
+      <c r="U15">
+        <v>19</v>
+      </c>
+      <c r="V15">
+        <v>8</v>
+      </c>
+      <c r="W15">
+        <v>3.5</v>
+      </c>
+      <c r="X15">
+        <v>0.65</v>
+      </c>
+      <c r="Y15">
+        <v>5.5</v>
+      </c>
+      <c r="Z15">
+        <v>0.75</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="16" spans="1:27" ht="20" x14ac:dyDescent="0.2">
-      <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="10:10" ht="20" x14ac:dyDescent="0.2">
-      <c r="J17" s="2"/>
-    </row>
-    <row r="18" spans="10:10" ht="20" x14ac:dyDescent="0.2">
-      <c r="J18" s="2"/>
-    </row>
-    <row r="24" spans="10:10" ht="20" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>175</v>
+      </c>
+      <c r="B16">
+        <v>71</v>
+      </c>
+      <c r="C16">
+        <v>51</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" t="s">
+        <v>43</v>
+      </c>
+      <c r="G16">
+        <v>0.108</v>
+      </c>
+      <c r="H16">
+        <v>5.6842109999999998E-3</v>
+      </c>
+      <c r="I16" s="2">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="J16" s="2">
+        <v>0.76670000000000005</v>
+      </c>
+      <c r="K16">
+        <v>100</v>
+      </c>
+      <c r="L16">
+        <v>100</v>
+      </c>
+      <c r="M16">
+        <v>100</v>
+      </c>
+      <c r="N16">
+        <v>0.2</v>
+      </c>
+      <c r="O16">
+        <v>50</v>
+      </c>
+      <c r="P16">
+        <v>50</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>10</v>
+      </c>
+      <c r="R16" t="s">
+        <v>10</v>
+      </c>
+      <c r="S16">
+        <v>8.5</v>
+      </c>
+      <c r="T16">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="U16">
+        <v>10.5</v>
+      </c>
+      <c r="V16">
+        <v>1.25</v>
+      </c>
+      <c r="W16">
+        <v>3.5</v>
+      </c>
+      <c r="X16">
+        <v>0.65</v>
+      </c>
+      <c r="Y16">
+        <v>5.5</v>
+      </c>
+      <c r="Z16">
+        <v>0.75</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" ht="20" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>176</v>
+      </c>
+      <c r="B17">
+        <v>71</v>
+      </c>
+      <c r="C17">
+        <v>51</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17">
+        <v>0.108</v>
+      </c>
+      <c r="H17">
+        <v>5.6842109999999998E-3</v>
+      </c>
+      <c r="I17" s="2">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="J17" s="2">
+        <v>0.76670000000000005</v>
+      </c>
+      <c r="K17">
+        <v>100</v>
+      </c>
+      <c r="L17">
+        <v>100</v>
+      </c>
+      <c r="M17">
+        <v>100</v>
+      </c>
+      <c r="N17">
+        <v>0.2</v>
+      </c>
+      <c r="O17">
+        <v>50</v>
+      </c>
+      <c r="P17">
+        <v>50</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>11</v>
+      </c>
+      <c r="R17" t="s">
+        <v>10</v>
+      </c>
+      <c r="S17">
+        <v>15.5</v>
+      </c>
+      <c r="T17">
+        <v>8</v>
+      </c>
+      <c r="U17">
+        <v>19</v>
+      </c>
+      <c r="V17">
+        <v>8</v>
+      </c>
+      <c r="W17">
+        <v>3.5</v>
+      </c>
+      <c r="X17">
+        <v>0.65</v>
+      </c>
+      <c r="Y17">
+        <v>5.5</v>
+      </c>
+      <c r="Z17">
+        <v>0.75</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" ht="20" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>177</v>
+      </c>
+      <c r="B18">
+        <v>51</v>
+      </c>
+      <c r="C18">
+        <v>30</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18">
+        <v>0.108</v>
+      </c>
+      <c r="H18">
+        <v>5.6842109999999998E-3</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="J18" s="2">
+        <v>0.76670000000000005</v>
+      </c>
+      <c r="K18">
+        <v>100</v>
+      </c>
+      <c r="L18">
+        <v>100</v>
+      </c>
+      <c r="M18">
+        <v>100</v>
+      </c>
+      <c r="N18">
+        <v>0.2</v>
+      </c>
+      <c r="O18">
+        <v>50</v>
+      </c>
+      <c r="P18">
+        <v>50</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>11</v>
+      </c>
+      <c r="R18" t="s">
+        <v>10</v>
+      </c>
+      <c r="S18">
+        <v>5</v>
+      </c>
+      <c r="T18">
+        <v>5</v>
+      </c>
+      <c r="U18">
+        <v>7</v>
+      </c>
+      <c r="V18">
+        <v>6.5</v>
+      </c>
+      <c r="W18">
+        <v>3.5</v>
+      </c>
+      <c r="X18">
+        <v>0.65</v>
+      </c>
+      <c r="Y18">
+        <v>5.5</v>
+      </c>
+      <c r="Z18">
+        <v>0.75</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" ht="20" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>178</v>
+      </c>
+      <c r="B19">
+        <v>71</v>
+      </c>
+      <c r="C19">
+        <v>51</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" t="s">
+        <v>43</v>
+      </c>
+      <c r="G19">
+        <v>0.108</v>
+      </c>
+      <c r="H19">
+        <v>5.6842109999999998E-3</v>
+      </c>
+      <c r="I19" s="2">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="J19" s="2">
+        <v>0.76670000000000005</v>
+      </c>
+      <c r="K19">
+        <v>100</v>
+      </c>
+      <c r="L19">
+        <v>100</v>
+      </c>
+      <c r="M19">
+        <v>100</v>
+      </c>
+      <c r="N19">
+        <v>0.2</v>
+      </c>
+      <c r="O19">
+        <v>50</v>
+      </c>
+      <c r="P19">
+        <v>50</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>11</v>
+      </c>
+      <c r="R19" t="s">
+        <v>10</v>
+      </c>
+      <c r="S19">
+        <v>5</v>
+      </c>
+      <c r="T19">
+        <v>5</v>
+      </c>
+      <c r="U19">
+        <v>7</v>
+      </c>
+      <c r="V19">
+        <v>6.5</v>
+      </c>
+      <c r="W19">
+        <v>3.5</v>
+      </c>
+      <c r="X19">
+        <v>0.65</v>
+      </c>
+      <c r="Y19">
+        <v>5.5</v>
+      </c>
+      <c r="Z19">
+        <v>0.75</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" ht="20" x14ac:dyDescent="0.2">
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="10:10" ht="20" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:27" ht="20" x14ac:dyDescent="0.2">
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="10:10" ht="20" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:27" ht="20" x14ac:dyDescent="0.2">
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="10:10" ht="20" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:27" ht="20" x14ac:dyDescent="0.2">
       <c r="J27" s="2"/>
     </row>
   </sheetData>
@@ -2609,7 +3110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DDB9334-8F56-FD47-AA9B-D960EB678BC9}">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="J55" sqref="A32:J55"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update runs to expand age structure (M = 0.065)
</commit_message>
<xml_diff>
--- a/input/OM_EM_Scenarios_v3.xlsx
+++ b/input/OM_EM_Scenarios_v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Fleet_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187491CF-4C88-E843-86FC-D3F03E58D6F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6D84D1-3560-DB4D-BFB3-25BE39554502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{7DE04263-F460-4046-B781-542FFAD9869D}"/>
+    <workbookView xWindow="2400" yWindow="880" windowWidth="30240" windowHeight="18880" xr2:uid="{7DE04263-F460-4046-B781-542FFAD9869D}"/>
   </bookViews>
   <sheets>
     <sheet name="OM" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="197">
   <si>
     <t>Fl_1_Ftype</t>
   </si>
@@ -622,6 +622,18 @@
   </si>
   <si>
     <t>Int_2Fl_GamL</t>
+  </si>
+  <si>
+    <t>Fast_LG_O_High_Ext</t>
+  </si>
+  <si>
+    <t>Fast_LG_Y_High_Ext</t>
+  </si>
+  <si>
+    <t>Fast_GL_O_High_Rev_Ext</t>
+  </si>
+  <si>
+    <t>Fast_GL_Y_High_Rev_Ext</t>
   </si>
 </sst>
 </file>
@@ -996,8 +1008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3458753E-37AB-3F45-AB3E-5A0862A1384B}">
   <dimension ref="A1:AA27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2603,6 +2615,338 @@
         <v>116</v>
       </c>
     </row>
+    <row r="20" spans="1:27" ht="20" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>193</v>
+      </c>
+      <c r="B20">
+        <v>100</v>
+      </c>
+      <c r="C20">
+        <v>30</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="H20">
+        <v>5.6842109999999998E-3</v>
+      </c>
+      <c r="I20" s="2">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="J20" s="2">
+        <v>0.76670000000000005</v>
+      </c>
+      <c r="K20">
+        <v>100</v>
+      </c>
+      <c r="L20">
+        <v>100</v>
+      </c>
+      <c r="M20">
+        <v>100</v>
+      </c>
+      <c r="N20">
+        <v>0.2</v>
+      </c>
+      <c r="O20">
+        <v>50</v>
+      </c>
+      <c r="P20">
+        <v>50</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>10</v>
+      </c>
+      <c r="R20" t="s">
+        <v>11</v>
+      </c>
+      <c r="S20">
+        <v>3.5</v>
+      </c>
+      <c r="T20">
+        <v>0.65</v>
+      </c>
+      <c r="U20">
+        <v>5.5</v>
+      </c>
+      <c r="V20">
+        <v>0.75</v>
+      </c>
+      <c r="W20">
+        <v>15.5</v>
+      </c>
+      <c r="X20">
+        <v>8</v>
+      </c>
+      <c r="Y20">
+        <v>19</v>
+      </c>
+      <c r="Z20">
+        <v>8</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" ht="20" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>194</v>
+      </c>
+      <c r="B21">
+        <v>100</v>
+      </c>
+      <c r="C21">
+        <v>30</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="H21">
+        <v>5.6842109999999998E-3</v>
+      </c>
+      <c r="I21" s="2">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="J21" s="2">
+        <v>0.76670000000000005</v>
+      </c>
+      <c r="K21">
+        <v>100</v>
+      </c>
+      <c r="L21">
+        <v>100</v>
+      </c>
+      <c r="M21">
+        <v>100</v>
+      </c>
+      <c r="N21">
+        <v>0.2</v>
+      </c>
+      <c r="O21">
+        <v>50</v>
+      </c>
+      <c r="P21">
+        <v>50</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>10</v>
+      </c>
+      <c r="R21" t="s">
+        <v>11</v>
+      </c>
+      <c r="S21">
+        <v>3.5</v>
+      </c>
+      <c r="T21">
+        <v>0.65</v>
+      </c>
+      <c r="U21">
+        <v>5.5</v>
+      </c>
+      <c r="V21">
+        <v>0.75</v>
+      </c>
+      <c r="W21">
+        <v>5</v>
+      </c>
+      <c r="X21">
+        <v>5</v>
+      </c>
+      <c r="Y21">
+        <v>7</v>
+      </c>
+      <c r="Z21">
+        <v>6.5</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" ht="20" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>195</v>
+      </c>
+      <c r="B22">
+        <v>100</v>
+      </c>
+      <c r="C22">
+        <v>30</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="H22">
+        <v>5.6842109999999998E-3</v>
+      </c>
+      <c r="I22" s="2">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="J22" s="2">
+        <v>0.76670000000000005</v>
+      </c>
+      <c r="K22">
+        <v>100</v>
+      </c>
+      <c r="L22">
+        <v>100</v>
+      </c>
+      <c r="M22">
+        <v>100</v>
+      </c>
+      <c r="N22">
+        <v>0.2</v>
+      </c>
+      <c r="O22">
+        <v>50</v>
+      </c>
+      <c r="P22">
+        <v>50</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>11</v>
+      </c>
+      <c r="R22" t="s">
+        <v>10</v>
+      </c>
+      <c r="S22">
+        <v>15.5</v>
+      </c>
+      <c r="T22">
+        <v>8</v>
+      </c>
+      <c r="U22">
+        <v>19</v>
+      </c>
+      <c r="V22">
+        <v>8</v>
+      </c>
+      <c r="W22">
+        <v>3.5</v>
+      </c>
+      <c r="X22">
+        <v>0.65</v>
+      </c>
+      <c r="Y22">
+        <v>5.5</v>
+      </c>
+      <c r="Z22">
+        <v>0.75</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" ht="20" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>196</v>
+      </c>
+      <c r="B23">
+        <v>100</v>
+      </c>
+      <c r="C23">
+        <v>30</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="H23">
+        <v>5.6842109999999998E-3</v>
+      </c>
+      <c r="I23" s="2">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="J23" s="2">
+        <v>0.76670000000000005</v>
+      </c>
+      <c r="K23">
+        <v>100</v>
+      </c>
+      <c r="L23">
+        <v>100</v>
+      </c>
+      <c r="M23">
+        <v>100</v>
+      </c>
+      <c r="N23">
+        <v>0.2</v>
+      </c>
+      <c r="O23">
+        <v>50</v>
+      </c>
+      <c r="P23">
+        <v>50</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>11</v>
+      </c>
+      <c r="R23" t="s">
+        <v>10</v>
+      </c>
+      <c r="S23">
+        <v>5</v>
+      </c>
+      <c r="T23">
+        <v>5</v>
+      </c>
+      <c r="U23">
+        <v>7</v>
+      </c>
+      <c r="V23">
+        <v>6.5</v>
+      </c>
+      <c r="W23">
+        <v>3.5</v>
+      </c>
+      <c r="X23">
+        <v>0.65</v>
+      </c>
+      <c r="Y23">
+        <v>5.5</v>
+      </c>
+      <c r="Z23">
+        <v>0.75</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>116</v>
+      </c>
+    </row>
     <row r="24" spans="1:27" ht="20" x14ac:dyDescent="0.2">
       <c r="J24" s="2"/>
     </row>
@@ -2625,7 +2969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5143D2C7-3A08-064F-9170-C1ED86770A52}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>

</xml_diff>